<commit_message>
alteracoes na pagina usuario
</commit_message>
<xml_diff>
--- a/documentacao/requisitos/requisitos funcionais, nao funcionais e regras de negocio.xlsx
+++ b/documentacao/requisitos/requisitos funcionais, nao funcionais e regras de negocio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Giovane\Magic World Bookstore\documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Giovane\Magic World Bookstore\documentacao\requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE217C4D-D6B7-4ED7-8ABD-06C4A5C7FBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6DF3C4-11D0-48E7-AED1-918416F28C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{919A8B89-A62A-49A5-AA3A-AC8B104AD212}"/>
   </bookViews>
@@ -22,23 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>RF001</t>
   </si>
@@ -137,6 +126,9 @@
   </si>
   <si>
     <t>Referente ao RF005, no momento da compra deve ser solicitado o endereço para entrega e a forma de pagamento. Caso seja cartão, solicitar o número do mesmo</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -201,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -211,12 +203,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -244,36 +235,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -590,7 +551,7 @@
   <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +562,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -616,7 +577,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -671,7 +632,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -682,7 +643,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -693,7 +654,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
@@ -704,7 +665,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
@@ -715,7 +676,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>